<commit_message>
# commit all scripts and generated files
</commit_message>
<xml_diff>
--- a/analysis/derived_data/MSTRdata.xlsx
+++ b/analysis/derived_data/MSTRdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t xml:space="preserve">Sample.ID</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t xml:space="preserve">4/13/2021 2:00:09 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naural</t>
   </si>
   <si>
     <t xml:space="preserve">14:57:58</t>
@@ -4015,7 +4012,7 @@
         <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -4027,10 +4024,10 @@
         <v>58</v>
       </c>
       <c r="H21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" t="s">
         <v>105</v>
-      </c>
-      <c r="I21" t="s">
-        <v>106</v>
       </c>
       <c r="J21" t="n">
         <v>255.4748064</v>
@@ -4184,10 +4181,10 @@
         <v>58</v>
       </c>
       <c r="H22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
         <v>107</v>
-      </c>
-      <c r="I22" t="s">
-        <v>108</v>
       </c>
       <c r="J22" t="n">
         <v>255.4748064</v>
@@ -4341,10 +4338,10 @@
         <v>58</v>
       </c>
       <c r="H23" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" t="s">
         <v>109</v>
-      </c>
-      <c r="I23" t="s">
-        <v>110</v>
       </c>
       <c r="J23" t="n">
         <v>255.4748064</v>
@@ -4498,10 +4495,10 @@
         <v>58</v>
       </c>
       <c r="H24" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" t="s">
         <v>111</v>
-      </c>
-      <c r="I24" t="s">
-        <v>112</v>
       </c>
       <c r="J24" t="n">
         <v>255.4748064</v>
@@ -4655,10 +4652,10 @@
         <v>58</v>
       </c>
       <c r="H25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" t="s">
         <v>113</v>
-      </c>
-      <c r="I25" t="s">
-        <v>114</v>
       </c>
       <c r="J25" t="n">
         <v>255.4748064</v>
@@ -4812,10 +4809,10 @@
         <v>58</v>
       </c>
       <c r="H26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" t="s">
         <v>115</v>
-      </c>
-      <c r="I26" t="s">
-        <v>116</v>
       </c>
       <c r="J26" t="n">
         <v>255.4748064</v>
@@ -4969,10 +4966,10 @@
         <v>58</v>
       </c>
       <c r="H27" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" t="s">
         <v>117</v>
-      </c>
-      <c r="I27" t="s">
-        <v>118</v>
       </c>
       <c r="J27" t="n">
         <v>255.4748064</v>
@@ -5124,10 +5121,10 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" t="s">
         <v>119</v>
-      </c>
-      <c r="I28" t="s">
-        <v>120</v>
       </c>
       <c r="J28" t="n">
         <v>255.4748064</v>
@@ -5279,10 +5276,10 @@
         <v>58</v>
       </c>
       <c r="H29" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" t="s">
         <v>121</v>
-      </c>
-      <c r="I29" t="s">
-        <v>122</v>
       </c>
       <c r="J29" t="n">
         <v>255.4748064</v>
@@ -5434,10 +5431,10 @@
         <v>58</v>
       </c>
       <c r="H30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" t="s">
         <v>123</v>
-      </c>
-      <c r="I30" t="s">
-        <v>124</v>
       </c>
       <c r="J30" t="n">
         <v>255.4748064</v>
@@ -5591,10 +5588,10 @@
         <v>58</v>
       </c>
       <c r="H31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" t="s">
         <v>125</v>
-      </c>
-      <c r="I31" t="s">
-        <v>126</v>
       </c>
       <c r="J31" t="n">
         <v>255.4748064</v>
@@ -5741,90 +5738,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
         <v>127</v>
-      </c>
-      <c r="B1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
         <v>129</v>
-      </c>
-      <c r="B2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
         <v>131</v>
-      </c>
-      <c r="B3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
         <v>133</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
         <v>139</v>
-      </c>
-      <c r="B9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
         <v>142</v>
-      </c>
-      <c r="B11" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12">
@@ -5832,7 +5829,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
@@ -5840,7 +5837,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14">
@@ -5848,7 +5845,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15">
@@ -5856,7 +5853,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16">
@@ -5864,7 +5861,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
@@ -5872,7 +5869,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18">
@@ -5880,55 +5877,55 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" t="s">
         <v>150</v>
-      </c>
-      <c r="B24" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="25">
@@ -5936,7 +5933,7 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26">
@@ -5944,159 +5941,159 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" t="s">
         <v>152</v>
-      </c>
-      <c r="B27" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" t="s">
         <v>161</v>
-      </c>
-      <c r="B35" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>